<commit_message>
DA18 | Day 8
</commit_message>
<xml_diff>
--- a/Batch/18/Day_8_Date_functions.xlsx
+++ b/Batch/18/Day_8_Date_functions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\Excel\Batch\17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\Excel\Batch\18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32208D0B-26C5-442D-8EEA-C6D384B2CC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466FBC86-2687-400B-A29D-71E5E226A329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
   <si>
     <t>Data Used in Formula</t>
   </si>
@@ -212,15 +212,6 @@
   </si>
   <si>
     <t>NETWORKDAY uses the start date and end date and returns the total working days. This does not includes weekends (Saturday and Sunday) and the specified holidays (d4:d6)</t>
-  </si>
-  <si>
-    <t>No Of Days</t>
-  </si>
-  <si>
-    <t>No Of working days considering Saturday and Sunday as weekend</t>
-  </si>
-  <si>
-    <t>No of Working days considering Monday as weekend</t>
   </si>
 </sst>
 </file>
@@ -5418,7 +5409,7 @@
       </c>
       <c r="C7" s="20">
         <f ca="1">NOW() +B3</f>
-        <v>45763.895796643519</v>
+        <v>45805.91914189815</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>32</v>
@@ -7535,10 +7526,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B1:E1000"/>
+  <dimension ref="B1:D1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7552,15 +7543,15 @@
     <col min="7" max="26" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="33"/>
       <c r="D2" s="33"/>
     </row>
-    <row r="3" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="5" t="s">
         <v>41</v>
       </c>
@@ -7571,7 +7562,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="21">
         <v>41699</v>
       </c>
@@ -7582,26 +7573,26 @@
         <v>41701</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
       <c r="D5" s="21">
         <v>41719</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
       <c r="D6" s="21">
         <v>41772</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="17"/>
     </row>
-    <row r="8" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="19" t="s">
         <v>1</v>
       </c>
@@ -7612,66 +7603,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="42" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="6"/>
       <c r="C9" s="27"/>
       <c r="D9" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="6"/>
       <c r="C10" s="27"/>
       <c r="D10" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="12"/>
-      <c r="C13" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13">
+      <c r="C13" s="28"/>
+    </row>
+    <row r="14" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="12"/>
+      <c r="C14" s="28">
         <f>C4-B4</f>
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="12"/>
-      <c r="C14" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14">
+    <row r="15" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="12"/>
+      <c r="C15" s="28">
         <f>NETWORKDAYS(B4,C4,D4:D6)</f>
         <v>68</v>
       </c>
-      <c r="E14">
-        <f>NETWORKDAYS(B4,C4)</f>
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="12"/>
-      <c r="C15" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15">
-        <f>NETWORKDAYS.INTL(B4,C4,12,D4:D6)</f>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="12"/>
+      <c r="C16">
+        <f>NETWORKDAYS.INTL(B4,C4,11,D4:D6)</f>
+        <v>83</v>
+      </c>
     </row>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>